<commit_message>
translation working - proof of concept
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/eu-dga.xlsx
+++ b/documentation-generator/vocab_csv/eu-dga.xlsx
@@ -305,7 +305,7 @@
     <t>Service provided by a data cooperative</t>
   </si>
   <si>
-    <t>dpv-dga:DataIntermediationService</t>
+    <t>eu-dga:DataIntermediationService</t>
   </si>
   <si>
     <t>DataIntermediationServiceBetweenHoldersUsers</t>
@@ -617,7 +617,7 @@
     <t>An entity constituted by data subjects, one-person undertakings or SMEs who provides data intermediation services and supports its members in the exercise of their data-related rights</t>
   </si>
   <si>
-    <t>dpv-dga:DISP</t>
+    <t>eu-dga:DISP</t>
   </si>
   <si>
     <t>DGA 2.15, 10.c</t>
@@ -728,7 +728,7 @@
     <t>An entity who is responsible for receiving and transmiting requests for the reuse of public data in the EU</t>
   </si>
   <si>
-    <t>dpv-dga:SIP</t>
+    <t>eu-dga:SIP</t>
   </si>
   <si>
     <t>DGA 8.4</t>
@@ -800,7 +800,7 @@
     <t>Indicates association with competent body designated by the Member State to assist Public Bodies in activities related to data reuse</t>
   </si>
   <si>
-    <t>dpv-dga:DataReuseAssistant</t>
+    <t>eu-dga:DataReuseAssistant</t>
   </si>
   <si>
     <t>dpv:hasEntity</t>
@@ -818,7 +818,7 @@
     <t>Indicates association with data user</t>
   </si>
   <si>
-    <t>dpv-dga:DataUser</t>
+    <t>eu-dga:DataUser</t>
   </si>
   <si>
     <t>hasDataHolder</t>
@@ -830,7 +830,7 @@
     <t>Indicates association with data holder</t>
   </si>
   <si>
-    <t>dpv-dga:DataHolder</t>
+    <t>eu-dga:DataHolder</t>
   </si>
   <si>
     <t>hasDAO</t>
@@ -842,7 +842,7 @@
     <t>Indicates association with data altruism organisation</t>
   </si>
   <si>
-    <t>dpv-dga:DataAltruismOrganisation</t>
+    <t>eu-dga:DataAltruismOrganisation</t>
   </si>
   <si>
     <t>hasDISP</t>

</xml_diff>